<commit_message>
- Update test case - Add new field "isActive" for Food and Table.
</commit_message>
<xml_diff>
--- a/Tags/Documents/Test Cases/Order Function Testing_10-1-2016.xlsx
+++ b/Tags/Documents/Test Cases/Order Function Testing_10-1-2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Order food</t>
   </si>
@@ -161,6 +161,54 @@
 9. Bàn 3 trở lại trạng thái trống, không hiển thị thời gian
 10. Báo cáo hiển thị bàn 3 đã bị hủy, đúng note</t>
   </si>
+  <si>
+    <t>Add new, edit, delete food | add new, edit, delete table</t>
+  </si>
+  <si>
+    <t>1. Thêm món cho bàn 1
+2. Vào supervisor thêm món "Trà đá vỉa hè" 5k và "Trà chanh chém gió" 10k
+3. Đặt thêm món "Trà đá vỉa hè" cho bàn 1
+4. Đặt thêm món "Trà chanh chém gió" cho bàn 1
+5. Vào supervisor sửa món "Trà chanh chém gió" thành "Trà chanh chém gió nhè nhẹ" và giá từ 10k lên 15k
+6. Thanh toán và Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>3. Món "Trà đá vỉa hè" hiển thị đúng trên order của bàn 1 và trong chức năng đặt món
+4. Món "Trà chanh chém gió" hiển thị đúng trên order của bàn 1 và trong chức năng đặt món
+5. Order của bàn 1 hiển thị đúng tên và số tiền
+6. Báo cáo xuất chính xác nội dung của đặt món của bàn 1</t>
+  </si>
+  <si>
+    <t>1. Thêm món cho bàn 1 có món "Trà đá vỉa hè" và "Trà chanh chém gió nhè nhẹ"
+2. Vào supervisor xóa món "Trà đá vỉa hè" và đổi tên "Trà chanh chém gió nhè nhè" thành "Trà chanh chém gió", 15k -&gt; 10k
+3. Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>2. Món trà đá vỉa hẻ đã xóa, tiền của món trà chanh chém gió giảm
+3. Báo cáo hiển thị đúng nội dung</t>
+  </si>
+  <si>
+    <t>1. Thêm bàn 101
+2. Đặt món cho bàn 101
+3. Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>3. Báo cáo hiển thị nội dung của bàn 101</t>
+  </si>
+  <si>
+    <t>1. Xóa bàn 101
+2. Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>2. Báo cáo vẫn phải hiển thị nội dung của bàn 101</t>
+  </si>
+  <si>
+    <t>- Đặt món A -&gt; vào supervisor xóa món A -&gt; Order hiện ra một order detail trắng ==&gt; Add state for food (enable | disable)</t>
+  </si>
+  <si>
+    <t>- Xóa bàn 11 -&gt; xuất báo cáo bị mất bàn 11 ==&gt; add state for table
+- Bàn 11 bị xóa nhưng chưa được reload</t>
+  </si>
 </sst>
 </file>
 
@@ -175,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,24 +255,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -232,6 +283,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,314 +573,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K26"/>
+  <dimension ref="A3:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="45.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="45.28515625" style="9" customWidth="1"/>
     <col min="8" max="8" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="291.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:8" ht="291.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:8" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="5" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+    <row r="9" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="5" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+    <row r="10" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="5" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="11" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="5" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="255" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+    <row r="12" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="5" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>16</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>17</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>18</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -841,8 +918,8 @@
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>

</xml_diff>

<commit_message>
- Update Test Cases/Order Function Testing_10-1-2016.xlsx
</commit_message>
<xml_diff>
--- a/Tags/Documents/Test Cases/Order Function Testing_10-1-2016.xlsx
+++ b/Tags/Documents/Test Cases/Order Function Testing_10-1-2016.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\WebApplication\Tags\Documents\Test Cases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="7380"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Order food</t>
   </si>
@@ -181,12 +186,60 @@
 13. Bàn hiển thị Order đúng số tiền, đúng danh sách các món, đúng note, hiển thị thông bán 1 đã đặt món
 14. Bàn hiển thị đang đợi 2 phút</t>
   </si>
+  <si>
+    <t>Add new, edit, delete food | add new, edit, delete table</t>
+  </si>
+  <si>
+    <t>1. Thêm món cho bàn 1
+2. Vào supervisor thêm món "Trà đá vỉa hè" 5k và "Trà chanh chém gió" 10k
+3. Đặt thêm món "Trà đá vỉa hè" cho bàn 1
+4. Đặt thêm món "Trà chanh chém gió" cho bàn 1
+5. Vào supervisor sửa món "Trà chanh chém gió" thành "Trà chanh chém gió nhè nhẹ" và giá từ 10k lên 15k
+6. Thanh toán và Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>3. Món "Trà đá vỉa hè" hiển thị đúng trên order của bàn 1 và trong chức năng đặt món
+4. Món "Trà chanh chém gió" hiển thị đúng trên order của bàn 1 và trong chức năng đặt món
+5. Order của bàn 1 hiển thị đúng tên và số tiền
+6. Báo cáo xuất chính xác nội dung của đặt món của bàn 1</t>
+  </si>
+  <si>
+    <t>1. Thêm món cho bàn 1 có món "Trà đá vỉa hè" và "Trà chanh chém gió nhè nhẹ"
+2. Vào supervisor xóa món "Trà đá vỉa hè" và đổi tên "Trà chanh chém gió nhè nhè" thành "Trà chanh chém gió", 15k -&gt; 10k
+3. Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>2. Món trà đá vỉa hẻ đã xóa, tiền của món trà chanh chém gió giảm
+3. Báo cáo hiển thị đúng nội dung</t>
+  </si>
+  <si>
+    <t>- Đặt món A -&gt; vào supervisor xóa món A -&gt; Order hiện ra một order detail trắng ==&gt; Add state for food (enable | disable)</t>
+  </si>
+  <si>
+    <t>1. Thêm bàn 101
+2. Đặt món cho bàn 101
+3. Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>3. Báo cáo hiển thị nội dung của bàn 101</t>
+  </si>
+  <si>
+    <t>- Xóa bàn 11 -&gt; xuất báo cáo bị mất bàn 11 ==&gt; add state for table
+- Bàn 11 bị xóa nhưng chưa được reload</t>
+  </si>
+  <si>
+    <t>1. Xóa bàn 101
+2. Xuất báo cáo</t>
+  </si>
+  <si>
+    <t>2. Báo cáo vẫn phải hiển thị nội dung của bàn 101</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +258,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -239,22 +298,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,21 +593,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="6" max="6" width="32" customWidth="1"/>
@@ -550,7 +615,7 @@
     <col min="8" max="8" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -565,7 +630,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -586,17 +651,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="291.75" customHeight="1">
+    <row r="5" spans="1:11" ht="291.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
@@ -607,17 +672,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="171.75" customHeight="1">
+    <row r="6" spans="1:11" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
@@ -625,17 +690,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1">
+    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
@@ -646,17 +711,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="59.25" customHeight="1">
+    <row r="8" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
@@ -664,17 +729,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="58.5" customHeight="1">
+    <row r="9" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
@@ -682,17 +747,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="99" customHeight="1">
+    <row r="10" spans="1:11" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
@@ -700,17 +765,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="100.5" customHeight="1">
+    <row r="11" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
@@ -718,183 +783,194 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="255">
+    <row r="12" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="2">
-        <v>9</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+    </row>
+    <row r="14" spans="1:11" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>10</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>11</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:11">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>12</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>13</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2">
-        <v>14</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2">
-        <v>15</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2">
-        <v>16</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2">
-        <v>17</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2">
-        <v>18</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
       <c r="G26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:F16"/>
@@ -907,6 +983,18 @@
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>